<commit_message>
se organiza algunos casos de prueba los archivos de autodiagnostico
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>ID Caso</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Validar cambios en la opcion Configuracion Wifi</t>
-  </si>
-  <si>
-    <t>El usuario debe haber accedido al apartado de información del cliente.</t>
   </si>
   <si>
     <t>1. Clic en módulo eCenter
@@ -145,6 +142,32 @@
   <si>
     <t>editar 
 configuracion de wifi</t>
+  </si>
+  <si>
+    <t>Redirigir ONT</t>
+  </si>
+  <si>
+    <t>Validar abrir modal redirigir ont y dar clic en la opcion "NO"</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion configuracion de wifi en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion Redirigir ONTen la lista de opciones</t>
+  </si>
+  <si>
+    <t>CP_AUTO_004</t>
+  </si>
+  <si>
+    <t>1. Clic en el boton OPCIONES
+2. Clic en opción “Redirigir ONT”
+3.Clic en el botón "NO" del modal de confirmación</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir cerrar el modal una vez se selecciona "NO"</t>
+  </si>
+  <si>
+    <t>El modal de redirigir ont se cierra correctamente.</t>
   </si>
 </sst>
 </file>
@@ -584,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -665,25 +688,25 @@
         <v>18</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="108" customHeight="1">
@@ -691,7 +714,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>15</v>
@@ -706,33 +729,33 @@
         <v>21</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="M3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="144.75" customHeight="1">
+    <row r="4" spans="1:13" ht="182.25" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>15</v>
@@ -744,28 +767,69 @@
         <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="M4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="144" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se ajusta en algunas vistas los casos de prueba del ingreso a la vista y se crean archivos de excel de casos de prueba.
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1B364-2DB7-4321-92B4-9E27E5EA578F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -24,9 +25,6 @@
     <t>ID Caso</t>
   </si>
   <si>
-    <t>Nombre Caso</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -169,12 +167,15 @@
   <si>
     <t>El modal de redirigir ont se cierra correctamente.</t>
   </si>
+  <si>
+    <t>Nombre/ Descripcion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -278,19 +279,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -315,9 +303,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -326,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,19 +594,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="5" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" customWidth="1"/>
     <col min="10" max="10" width="22.140625" customWidth="1"/>
@@ -627,209 +615,209 @@
     <col min="13" max="13" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="35.25" customHeight="1">
+    <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="114" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:13" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>25</v>
+      <c r="M3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="108" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="4" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>25</v>
+      <c r="M4" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="182.25" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="9" t="s">
+    <row r="5" spans="1:13" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="G5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="144" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="M5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se crea el caso de prueba CP_GESCLSERDOM_003 en gestion de clientes y servicios domiciliarios
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1B364-2DB7-4321-92B4-9E27E5EA578F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB201DE1-C23E-4774-A6A4-3C4FD7C27168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>ID Caso</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>Módulo</t>
   </si>
   <si>
-    <t>Descripción del Caso de Prueba</t>
-  </si>
-  <si>
     <t>Precondiciones</t>
   </si>
   <si>
@@ -70,25 +64,16 @@
     <t>eCenter</t>
   </si>
   <si>
-    <t>Validar el ingreso a la vista “Autodiagnostico” y se muestre la información correctamente</t>
-  </si>
-  <si>
     <t>El usuario debe tener permisos para acceder a la vista</t>
   </si>
   <si>
     <t>CP_AUTO_002</t>
   </si>
   <si>
-    <t>Validar la consulta del cliente de autodiagnostico por ID DEAL</t>
-  </si>
-  <si>
     <t>El usuario debe haber accedido a la vista de Autodiagnostico.</t>
   </si>
   <si>
     <t>CP_AUTO_003</t>
-  </si>
-  <si>
-    <t>Validar cambios en la opcion Configuracion Wifi</t>
   </si>
   <si>
     <t>1. Clic en módulo eCenter
@@ -145,9 +130,6 @@
     <t>Redirigir ONT</t>
   </si>
   <si>
-    <t>Validar abrir modal redirigir ont y dar clic en la opcion "NO"</t>
-  </si>
-  <si>
     <t>El usuario debe haber seleccionado la opcion configuracion de wifi en la lista de opciones</t>
   </si>
   <si>
@@ -169,6 +151,9 @@
   </si>
   <si>
     <t>Nombre/ Descripcion</t>
+  </si>
+  <si>
+    <t>Tipo de prueba</t>
   </si>
 </sst>
 </file>
@@ -595,229 +580,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="5" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="32.140625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="B4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="144" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se ajusta código y documento e unas vistas
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB201DE1-C23E-4774-A6A4-3C4FD7C27168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>ID Caso</t>
   </si>
@@ -155,12 +154,42 @@
   <si>
     <t>Tipo de prueba</t>
   </si>
+  <si>
+    <t>creacion de ordenes</t>
+  </si>
+  <si>
+    <t>CP_AUTO_005</t>
+  </si>
+  <si>
+    <t>CP_AUTO_006</t>
+  </si>
+  <si>
+    <t>funcion UPnP</t>
+  </si>
+  <si>
+    <t>CP_AUTO_007</t>
+  </si>
+  <si>
+    <t>funcion DMZ</t>
+  </si>
+  <si>
+    <t>CP_AUTO_008</t>
+  </si>
+  <si>
+    <t>ipv4 port Mapping</t>
+  </si>
+  <si>
+    <t>CP_AUTO_009</t>
+  </si>
+  <si>
+    <t>reserva DHCP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,14 +608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -601,7 +630,7 @@
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="114" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -677,7 +706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="108" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -715,7 +744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -753,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="144" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -788,6 +817,146 @@
         <v>22</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="51.75" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="36.75" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="39.75" customHeight="1">
+      <c r="A8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="39.75" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agregaron los casos de prueba al codigo de autodiagnostico, realizar ajustes del codigo
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A121C-6D0A-45FD-A928-5DD50D1823A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>ID Caso</t>
   </si>
@@ -184,12 +185,18 @@
   <si>
     <t>reserva DHCP</t>
   </si>
+  <si>
+    <t>CP_AUTO_010</t>
+  </si>
+  <si>
+    <t>Dispositivos conectados</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,14 +615,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -630,7 +637,7 @@
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1">
+    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -706,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -744,7 +751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -782,7 +789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1">
+    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -820,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51.75" customHeight="1">
+    <row r="6" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
@@ -848,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="36.75" customHeight="1">
+    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
@@ -876,7 +883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="39.75" customHeight="1">
+    <row r="8" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
@@ -904,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="39.75" customHeight="1">
+    <row r="9" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>47</v>
       </c>
@@ -932,7 +939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
@@ -960,6 +967,34 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se ajusta algunos casos de prueba en contenido clases negocio
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2A121C-6D0A-45FD-A928-5DD50D1823A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1157853-FA95-4A10-9F62-995087227669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se agregan casos de prueba en los doc y se agregan casos de prueba en contenido clases de negocio
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1157853-FA95-4A10-9F62-995087227669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F5B3D8-9A30-4858-8358-CA3ED5AEF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -326,9 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -618,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +638,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -717,7 +714,7 @@
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -755,7 +752,7 @@
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -793,7 +790,7 @@
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -831,7 +828,7 @@
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -859,7 +856,7 @@
       <c r="A7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -887,7 +884,7 @@
       <c r="A8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -915,7 +912,7 @@
       <c r="A9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -939,11 +936,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -967,11 +964,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="4" t="s">

</xml_diff>

<commit_message>
se agregan cambios en autodiagnostico en codigo y excel, otros cambios en explorador entidades
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F5B3D8-9A30-4858-8358-CA3ED5AEF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>ID Caso</t>
   </si>
@@ -108,95 +107,136 @@
 3. Clic en el botón "Consultar cliente"</t>
   </si>
   <si>
+    <t>La vista Autodiagnóstico se cargó sin errores</t>
+  </si>
+  <si>
+    <t>La información del usuario se mostró completa</t>
+  </si>
+  <si>
+    <t>Se actualizaron correctamente el nombre de la red y la contraseña se validó que los cambios se guardan.</t>
+  </si>
+  <si>
+    <t>editar 
+configuracion de wifi</t>
+  </si>
+  <si>
+    <t>Redirigir ONT</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion configuracion de wifi en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion Redirigir ONTen la lista de opciones</t>
+  </si>
+  <si>
+    <t>CP_AUTO_004</t>
+  </si>
+  <si>
+    <t>1. Clic en el boton OPCIONES
+2. Clic en opción “Redirigir ONT”
+3.Clic en el botón "NO" del modal de confirmación</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir cerrar el modal una vez se selecciona "NO"</t>
+  </si>
+  <si>
+    <t>El modal de redirigir ont se cierra correctamente.</t>
+  </si>
+  <si>
+    <t>Nombre/ Descripcion</t>
+  </si>
+  <si>
+    <t>Tipo de prueba</t>
+  </si>
+  <si>
+    <t>creacion de ordenes</t>
+  </si>
+  <si>
+    <t>CP_AUTO_005</t>
+  </si>
+  <si>
+    <t>CP_AUTO_006</t>
+  </si>
+  <si>
+    <t>funcion UPnP</t>
+  </si>
+  <si>
+    <t>CP_AUTO_007</t>
+  </si>
+  <si>
+    <t>funcion DMZ</t>
+  </si>
+  <si>
+    <t>CP_AUTO_008</t>
+  </si>
+  <si>
+    <t>ipv4 port Mapping</t>
+  </si>
+  <si>
+    <t>CP_AUTO_009</t>
+  </si>
+  <si>
+    <t>reserva DHCP</t>
+  </si>
+  <si>
+    <t>CP_AUTO_010</t>
+  </si>
+  <si>
+    <t>Dispositivos conectados</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion creacion de ordenes en la lista de opciones</t>
+  </si>
+  <si>
     <t>1. Clic en el boton OPCIONES
 2. Clic en opción "Configuración WiFi"
 3. Seleccionar el campo "Nombre de red"
-4.Digitar "TEST_EDICION" en el campo "Nombre de red"</t>
-  </si>
-  <si>
-    <t>La vista Autodiagnóstico se cargó sin errores</t>
-  </si>
-  <si>
-    <t>La información del usuario se mostró completa</t>
-  </si>
-  <si>
-    <t>Se actualizaron correctamente el nombre de la red y la contraseña se validó que los cambios se guardan.</t>
-  </si>
-  <si>
-    <t>editar 
-configuracion de wifi</t>
-  </si>
-  <si>
-    <t>Redirigir ONT</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion configuracion de wifi en la lista de opciones</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion Redirigir ONTen la lista de opciones</t>
-  </si>
-  <si>
-    <t>CP_AUTO_004</t>
-  </si>
-  <si>
-    <t>1. Clic en el boton OPCIONES
-2. Clic en opción “Redirigir ONT”
-3.Clic en el botón "NO" del modal de confirmación</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir cerrar el modal una vez se selecciona "NO"</t>
-  </si>
-  <si>
-    <t>El modal de redirigir ont se cierra correctamente.</t>
-  </si>
-  <si>
-    <t>Nombre/ Descripcion</t>
-  </si>
-  <si>
-    <t>Tipo de prueba</t>
-  </si>
-  <si>
-    <t>creacion de ordenes</t>
-  </si>
-  <si>
-    <t>CP_AUTO_005</t>
-  </si>
-  <si>
-    <t>CP_AUTO_006</t>
-  </si>
-  <si>
-    <t>funcion UPnP</t>
-  </si>
-  <si>
-    <t>CP_AUTO_007</t>
-  </si>
-  <si>
-    <t>funcion DMZ</t>
-  </si>
-  <si>
-    <t>CP_AUTO_008</t>
-  </si>
-  <si>
-    <t>ipv4 port Mapping</t>
-  </si>
-  <si>
-    <t>CP_AUTO_009</t>
-  </si>
-  <si>
-    <t>reserva DHCP</t>
-  </si>
-  <si>
-    <t>CP_AUTO_010</t>
-  </si>
-  <si>
-    <t>Dispositivos conectados</t>
+4. Digitar nuevo nombre de red
+5. Clic en el select CANAL
+6. Selección aleatoria de canal
+7. Clic en select ANCHO BANDA CANAL
+8. Selección aleatoria de ancho de banda
+9. Marcar checkbox 'Unsecured'
+10. Clic en botón ENVIAR y esperar progress
+11.Cerrar modal de Configuración WiFi</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Clic en opción "Creación de órdenes"
+3.Clic en el select "Tipo de orden"
+4.eleccionar opción "Orden de mantenimiento"
+5.Clic en el select "Posible falla"
+6.Seleccionar opción aleatoria en "Posible falla"
+7.Diligenciar campo "Observaciones".
+8.Clic en botón "Generar orden"
+9.Clic en botón "Sí" del modal de confirmación</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion funcion UPnP en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion funcion DMZ en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion ipv4 port Mapping en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion reserva DHCP en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion Dispositivos conectados en la lista de opciones</t>
+  </si>
+  <si>
+    <t>1. Clic en botón "Opciones"
+2.Clic en opción "funcion UPnP"
+3.Clic en Botón Cancelar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +252,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -307,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -332,6 +379,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,37 +662,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:L2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -672,7 +723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="114" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -698,7 +749,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>21</v>
@@ -710,7 +761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="108" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -736,7 +787,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>21</v>
@@ -748,12 +799,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>12</v>
@@ -762,10 +813,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -774,7 +825,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>21</v>
@@ -786,12 +837,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="144" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -800,19 +851,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>21</v>
@@ -824,12 +875,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="171" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>12</v>
@@ -837,9 +888,15 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
@@ -852,12 +909,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="89.25" customHeight="1">
       <c r="A7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
@@ -865,9 +922,15 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
@@ -880,12 +943,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="58.5" customHeight="1">
       <c r="A8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -893,7 +956,9 @@
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -908,12 +973,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="57.75" customHeight="1">
       <c r="A9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
@@ -921,7 +986,9 @@
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -936,12 +1003,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="57" customHeight="1">
       <c r="A10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>12</v>
@@ -949,7 +1016,9 @@
       <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -964,12 +1033,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="49.5" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>12</v>
@@ -977,7 +1046,9 @@
       <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -994,5 +1065,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se realizan ajustes en autodiagnostico archivo y excel
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A47E4-129E-4827-A9EA-235608855659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
   <si>
     <t>ID Caso</t>
   </si>
@@ -231,12 +232,52 @@
 2.Clic en opción "funcion UPnP"
 3.Clic en Botón Cancelar</t>
   </si>
+  <si>
+    <t>1.Clic en Botón Opciones
+2.Clic en Opción DMZ
+3.Clic casilla Habilitar DMZ
+4.Diligenciar IP aleatoria
+5.Clic en Botón Refrescar
+6.Clic en Botón Cancelar
+7.</t>
+  </si>
+  <si>
+    <t>1.Botón "Opciones"
+2.Opción "IPv4 Port Mapping"
+3.Clic en el campo "Protocolo"
+4.Seleccionar opción aleatoria en "Protocolo"
+5.Diligenciar campo "Dirección IP" con una IPv4 aleatoria
+6.Clic en botón "Refrescar"
+7.Clic en botón "Cancelar"</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Clic en Opción "Reserva DHCP"
+3.Diligenciar MAC aleatoria
+4.Diligenciar IPv4 aleatoria
+5.Clic en botón "Refrescar"
+6.Clic en botón "Cancelar"</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Opción "Dispositivos Conectados"
+3.Clic en flecha desplegable del primer dispositivo
+4.Clic en flecha desplegable del segundo dispositivo
+5.Clic en botón "Recargar/Refrescar"
+6.Cerrar modal "Dispositivos Conectados"</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir la creacion de la orden</t>
+  </si>
+  <si>
+    <t>La orden se crea correctamente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,14 +703,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -685,7 +726,7 @@
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1">
+    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -761,7 +802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -799,7 +840,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -837,7 +878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1">
+    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -875,7 +916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="171" customHeight="1">
+    <row r="6" spans="1:12" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
@@ -897,8 +938,12 @@
       <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="J6" s="3" t="s">
         <v>21</v>
       </c>
@@ -909,7 +954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="89.25" customHeight="1">
+    <row r="7" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -943,7 +988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1">
+    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -959,8 +1004,12 @@
       <c r="E8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
@@ -973,7 +1022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="57.75" customHeight="1">
+    <row r="9" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
@@ -989,8 +1038,12 @@
       <c r="E9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
@@ -1003,7 +1056,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="57" customHeight="1">
+    <row r="10" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
@@ -1019,8 +1072,12 @@
       <c r="E10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
@@ -1033,7 +1090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="49.5" customHeight="1">
+    <row r="11" spans="1:12" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -1049,8 +1106,12 @@
       <c r="E11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">

</xml_diff>

<commit_message>
se realizar ajustes en documento y codigo en contenidoClasesNegocio y autodiagnostico
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A47E4-129E-4827-A9EA-235608855659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t>ID Caso</t>
   </si>
@@ -272,12 +271,24 @@
   <si>
     <t>La orden se crea correctamente</t>
   </si>
+  <si>
+    <t>El modal se abre correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir abrir el modal</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir abrir el modal y mostrar la información</t>
+  </si>
+  <si>
+    <t>El modal se abre y muestra la información correctamente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,14 +714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -726,7 +737,7 @@
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -764,7 +775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="114" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -802,7 +813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="108" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -840,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -878,7 +889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="144" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -916,7 +927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="171" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
@@ -954,7 +965,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="89.25" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
@@ -976,8 +987,12 @@
       <c r="G7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="58.5" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>44</v>
       </c>
@@ -1010,8 +1025,12 @@
       <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1022,7 +1041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="142.5" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>46</v>
       </c>
@@ -1044,8 +1063,12 @@
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="J9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1056,7 +1079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="85.5" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
@@ -1078,8 +1101,12 @@
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1090,7 +1117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="134.25" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>50</v>
       </c>
@@ -1112,8 +1139,12 @@
       <c r="G11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="J11" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
se realizan ajustes en algunos archivo en codigo, excel y diagrama
</commit_message>
<xml_diff>
--- a/docs/test-cases/autodiagnostico.xlsx
+++ b/docs/test-cases/autodiagnostico.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73E470F-A269-4C55-817C-97D83A819971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autodiagnostico" sheetId="1" r:id="rId1"/>
@@ -102,11 +103,6 @@
 ID DEAL</t>
   </si>
   <si>
-    <t>1. Clic en el boton ID DEAL
-2. Ingresar número ID DEAL válido
-3. Clic en el botón "Consultar cliente"</t>
-  </si>
-  <si>
     <t>La vista Autodiagnóstico se cargó sin errores</t>
   </si>
   <si>
@@ -158,27 +154,15 @@
     <t>CP_AUTO_006</t>
   </si>
   <si>
-    <t>funcion UPnP</t>
-  </si>
-  <si>
     <t>CP_AUTO_007</t>
   </si>
   <si>
-    <t>funcion DMZ</t>
-  </si>
-  <si>
     <t>CP_AUTO_008</t>
   </si>
   <si>
-    <t>ipv4 port Mapping</t>
-  </si>
-  <si>
     <t>CP_AUTO_009</t>
   </si>
   <si>
-    <t>reserva DHCP</t>
-  </si>
-  <si>
     <t>CP_AUTO_010</t>
   </si>
   <si>
@@ -186,6 +170,94 @@
   </si>
   <si>
     <t>El usuario debe haber seleccionado la opcion creacion de ordenes en la lista de opciones</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Clic en opción "Creación de órdenes"
+3.Clic en el select "Tipo de orden"
+4.eleccionar opción "Orden de mantenimiento"
+5.Clic en el select "Posible falla"
+6.Seleccionar opción aleatoria en "Posible falla"
+7.Diligenciar campo "Observaciones".
+8.Clic en botón "Generar orden"
+9.Clic en botón "Sí" del modal de confirmación</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion funcion UPnP en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion funcion DMZ en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion ipv4 port Mapping en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion reserva DHCP en la lista de opciones</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado la opcion Dispositivos conectados en la lista de opciones</t>
+  </si>
+  <si>
+    <t>1. Clic en botón "Opciones"
+2.Clic en opción "funcion UPnP"
+3.Clic en Botón Cancelar</t>
+  </si>
+  <si>
+    <t>1.Clic en Botón Opciones
+2.Clic en Opción DMZ
+3.Clic casilla Habilitar DMZ
+4.Diligenciar IP aleatoria
+5.Clic en Botón Refrescar
+6.Clic en Botón Cancelar
+7.</t>
+  </si>
+  <si>
+    <t>1.Botón "Opciones"
+2.Opción "IPv4 Port Mapping"
+3.Clic en el campo "Protocolo"
+4.Seleccionar opción aleatoria en "Protocolo"
+5.Diligenciar campo "Dirección IP" con una IPv4 aleatoria
+6.Clic en botón "Refrescar"
+7.Clic en botón "Cancelar"</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Clic en Opción "Reserva DHCP"
+3.Diligenciar MAC aleatoria
+4.Diligenciar IPv4 aleatoria
+5.Clic en botón "Refrescar"
+6.Clic en botón "Cancelar"</t>
+  </si>
+  <si>
+    <t>1.Clic en botón "Opciones"
+2.Opción "Dispositivos Conectados"
+3.Clic en flecha desplegable del primer dispositivo
+4.Clic en flecha desplegable del segundo dispositivo
+5.Clic en botón "Recargar/Refrescar"
+6.Cerrar modal "Dispositivos Conectados"</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir la creacion de la orden</t>
+  </si>
+  <si>
+    <t>La orden se crea correctamente</t>
+  </si>
+  <si>
+    <t>El modal se abre correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir abrir el modal</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir abrir el modal y mostrar la información</t>
+  </si>
+  <si>
+    <t>El modal se abre y muestra la información correctamente</t>
+  </si>
+  <si>
+    <t>1. Clic en el boton ID DEAL
+2. Ingresar número ID DEAL válido
+3. clic en Consultar cliente</t>
   </si>
   <si>
     <t>1. Clic en el boton OPCIONES
@@ -198,97 +270,26 @@
 8. Selección aleatoria de ancho de banda
 9. Marcar checkbox 'Unsecured'
 10. Clic en botón ENVIAR y esperar progress
-11.Cerrar modal de Configuración WiFi</t>
-  </si>
-  <si>
-    <t>1.Clic en botón "Opciones"
-2.Clic en opción "Creación de órdenes"
-3.Clic en el select "Tipo de orden"
-4.eleccionar opción "Orden de mantenimiento"
-5.Clic en el select "Posible falla"
-6.Seleccionar opción aleatoria en "Posible falla"
-7.Diligenciar campo "Observaciones".
-8.Clic en botón "Generar orden"
-9.Clic en botón "Sí" del modal de confirmación</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion funcion UPnP en la lista de opciones</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion funcion DMZ en la lista de opciones</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion ipv4 port Mapping en la lista de opciones</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion reserva DHCP en la lista de opciones</t>
-  </si>
-  <si>
-    <t>El usuario debe haber seleccionado la opcion Dispositivos conectados en la lista de opciones</t>
-  </si>
-  <si>
-    <t>1. Clic en botón "Opciones"
-2.Clic en opción "funcion UPnP"
-3.Clic en Botón Cancelar</t>
-  </si>
-  <si>
-    <t>1.Clic en Botón Opciones
-2.Clic en Opción DMZ
-3.Clic casilla Habilitar DMZ
-4.Diligenciar IP aleatoria
-5.Clic en Botón Refrescar
-6.Clic en Botón Cancelar
-7.</t>
-  </si>
-  <si>
-    <t>1.Botón "Opciones"
-2.Opción "IPv4 Port Mapping"
-3.Clic en el campo "Protocolo"
-4.Seleccionar opción aleatoria en "Protocolo"
-5.Diligenciar campo "Dirección IP" con una IPv4 aleatoria
-6.Clic en botón "Refrescar"
-7.Clic en botón "Cancelar"</t>
-  </si>
-  <si>
-    <t>1.Clic en botón "Opciones"
-2.Clic en Opción "Reserva DHCP"
-3.Diligenciar MAC aleatoria
-4.Diligenciar IPv4 aleatoria
-5.Clic en botón "Refrescar"
-6.Clic en botón "Cancelar"</t>
-  </si>
-  <si>
-    <t>1.Clic en botón "Opciones"
-2.Opción "Dispositivos Conectados"
-3.Clic en flecha desplegable del primer dispositivo
-4.Clic en flecha desplegable del segundo dispositivo
-5.Clic en botón "Recargar/Refrescar"
-6.Cerrar modal "Dispositivos Conectados"</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir la creacion de la orden</t>
-  </si>
-  <si>
-    <t>La orden se crea correctamente</t>
-  </si>
-  <si>
-    <t>El modal se abre correctamente</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir abrir el modal</t>
-  </si>
-  <si>
-    <t>El sistema debe permitir abrir el modal y mostrar la información</t>
-  </si>
-  <si>
-    <t>El modal se abre y muestra la información correctamente</t>
+11. Cerrar modal de Configuración WiFi</t>
+  </si>
+  <si>
+    <t>funcion UPnP(opcion click boton cancelar)</t>
+  </si>
+  <si>
+    <t>funcion DMZ(opcion click boton cancelar)</t>
+  </si>
+  <si>
+    <t>ipv4 port Mapping(opcion click boton cancelar)</t>
+  </si>
+  <si>
+    <t>reserva DHCP(opcion click boton cancelar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,14 +715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -737,15 +738,15 @@
     <col min="12" max="12" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.25" customHeight="1">
+    <row r="1" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -775,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="114" customHeight="1">
+    <row r="2" spans="1:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -801,7 +802,7 @@
         <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>21</v>
@@ -813,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="108" customHeight="1">
+    <row r="3" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -830,7 +831,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>19</v>
@@ -839,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>21</v>
@@ -851,12 +852,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="182.25" customHeight="1">
+    <row r="4" spans="1:12" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>12</v>
@@ -865,10 +866,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>19</v>
@@ -877,7 +878,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>21</v>
@@ -889,12 +890,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="144" customHeight="1">
+    <row r="5" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -903,19 +904,19 @@
         <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>21</v>
@@ -927,12 +928,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="171" customHeight="1">
+    <row r="6" spans="1:12" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>12</v>
@@ -941,19 +942,19 @@
         <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>21</v>
@@ -965,12 +966,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="89.25" customHeight="1">
+    <row r="7" spans="1:12" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>12</v>
@@ -979,19 +980,19 @@
         <v>13</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>21</v>
@@ -1003,12 +1004,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1">
+    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -1017,19 +1018,19 @@
         <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
@@ -1041,12 +1042,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="142.5" customHeight="1">
+    <row r="9" spans="1:12" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>12</v>
@@ -1055,19 +1056,19 @@
         <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>21</v>
@@ -1079,12 +1080,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="85.5" customHeight="1">
+    <row r="10" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>12</v>
@@ -1093,19 +1094,19 @@
         <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>21</v>
@@ -1117,12 +1118,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="134.25" customHeight="1">
+    <row r="11" spans="1:12" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>12</v>
@@ -1131,19 +1132,19 @@
         <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>21</v>

</xml_diff>